<commit_message>
Added buggy auto trialing
it only goes up to 1, 2, then instead of 3 => 2 ?
</commit_message>
<xml_diff>
--- a/sum.xlsx
+++ b/sum.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qedu-my.sharepoint.com/personal/mcart226_eq_edu_au/Documents/School/EE/Thrust Stand/Thrust Stand Code/Arduino_Thrust_Stand/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_2B59D2BFD3E0D7087C7A9A504C3088B35299F7A4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_2B59D2BFD3D0D221DB9A271159F7E03348B3FB0F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F98ACC61-E716-974F-9146-752AD681D902}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -389,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B20" sqref="B20:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -410,7 +423,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1.0740000000000001</v>
+        <v>1.194</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -418,7 +431,7 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>8.6999999999999994E-2</v>
+        <v>2.956</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -426,7 +439,7 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>2.7879999999999998</v>
+        <v>5.2329999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -434,7 +447,7 @@
         <v>40</v>
       </c>
       <c r="B5">
-        <v>3.7709999999999999</v>
+        <v>6.5190000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -442,7 +455,7 @@
         <v>50</v>
       </c>
       <c r="B6">
-        <v>4.7249999999999996</v>
+        <v>7.7960000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -450,7 +463,7 @@
         <v>60</v>
       </c>
       <c r="B7">
-        <v>5.532</v>
+        <v>9.266</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -458,7 +471,7 @@
         <v>70</v>
       </c>
       <c r="B8">
-        <v>6.43</v>
+        <v>11.484</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -466,7 +479,7 @@
         <v>80</v>
       </c>
       <c r="B9">
-        <v>7.274</v>
+        <v>12.997</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -474,7 +487,7 @@
         <v>90</v>
       </c>
       <c r="B10">
-        <v>7.5419999999999998</v>
+        <v>13.747999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -482,7 +495,7 @@
         <v>100</v>
       </c>
       <c r="B11">
-        <v>8.1530000000000005</v>
+        <v>14.923</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -490,7 +503,7 @@
         <v>110</v>
       </c>
       <c r="B12">
-        <v>8.59</v>
+        <v>15.29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -498,7 +511,7 @@
         <v>120</v>
       </c>
       <c r="B13">
-        <v>9.2680000000000007</v>
+        <v>16.823</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -506,7 +519,7 @@
         <v>130</v>
       </c>
       <c r="B14">
-        <v>9.4789999999999992</v>
+        <v>16.861999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -514,7 +527,7 @@
         <v>140</v>
       </c>
       <c r="B15">
-        <v>10.151999999999999</v>
+        <v>17.757000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -522,7 +535,7 @@
         <v>150</v>
       </c>
       <c r="B16">
-        <v>10.705</v>
+        <v>18.099</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -530,7 +543,7 @@
         <v>160</v>
       </c>
       <c r="B17">
-        <v>11.717000000000001</v>
+        <v>18.61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -538,7 +551,7 @@
         <v>170</v>
       </c>
       <c r="B18">
-        <v>13.061999999999999</v>
+        <v>20.411000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -546,7 +559,151 @@
         <v>180</v>
       </c>
       <c r="B19">
-        <v>14.64</v>
+        <v>20.759</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>1.1779999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3.0089999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>4.391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23">
+        <v>6.194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>7.9630000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>60</v>
+      </c>
+      <c r="B25">
+        <v>9.3490000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>70</v>
+      </c>
+      <c r="B26">
+        <v>12.484999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>80</v>
+      </c>
+      <c r="B27">
+        <v>12.958</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>90</v>
+      </c>
+      <c r="B28">
+        <v>13.954000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>100</v>
+      </c>
+      <c r="B29">
+        <v>14.804</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>110</v>
+      </c>
+      <c r="B30">
+        <v>15.574</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>120</v>
+      </c>
+      <c r="B31">
+        <v>16.187000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>130</v>
+      </c>
+      <c r="B32">
+        <v>16.945</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>140</v>
+      </c>
+      <c r="B33">
+        <v>17.532</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>150</v>
+      </c>
+      <c r="B34">
+        <v>18.402999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>160</v>
+      </c>
+      <c r="B35">
+        <v>18.427</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>170</v>
+      </c>
+      <c r="B36">
+        <v>20.405999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>180</v>
+      </c>
+      <c r="B37">
+        <v>19.887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>